<commit_message>
Add HQC and Kyber post-quantum algorithm projects
Initial commit of HQC and Kyber post-quantum cryptography projects for PSoC ModusToolbox. Includes source code, headers, build files, board support packages, documentation, and configuration for the CY8CPROTO-063-BLE platform.
</commit_message>
<xml_diff>
--- a/Tests/Resumen.xlsx
+++ b/Tests/Resumen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bogur\Documents\GitHub\TFG2\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bogurad\Desktop\ProyectosgitHub\TFG2\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EDE3629-DC11-42A6-B6D4-A545D7E39AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD76BA5-FF06-4F77-BD7B-41EEBA4026A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBF9A5E8-AF43-43E1-A355-BBD13C05A84A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>HQC</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>Operations 1 Second</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Stack Depth (bytes)</t>
@@ -84,10 +81,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -455,7 +458,7 @@
   <dimension ref="A2:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,8 +513,8 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
+      <c r="C4" s="1">
+        <v>571896356</v>
       </c>
       <c r="D4">
         <v>22894712</v>
@@ -542,8 +545,8 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
+      <c r="C5" s="1">
+        <v>1148267355</v>
       </c>
       <c r="D5">
         <v>44027046</v>
@@ -574,8 +577,8 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
+      <c r="C6" s="1">
+        <v>1743477982</v>
       </c>
       <c r="D6">
         <v>67662397</v>
@@ -609,8 +612,8 @@
       <c r="B7" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
+      <c r="C7" s="1">
+        <v>1</v>
       </c>
       <c r="D7">
         <v>99</v>
@@ -641,8 +644,8 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>11</v>
+      <c r="C8" s="1">
+        <v>1</v>
       </c>
       <c r="D8">
         <v>51</v>
@@ -673,8 +676,8 @@
       <c r="B9" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
+      <c r="C9" s="1">
+        <v>1</v>
       </c>
       <c r="D9">
         <v>33</v>
@@ -703,13 +706,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>11</v>
+      <c r="C10" s="1">
+        <v>103596</v>
       </c>
       <c r="D10">
         <v>102688</v>
@@ -740,8 +743,8 @@
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>11</v>
+      <c r="C11" s="1">
+        <v>161364</v>
       </c>
       <c r="D11">
         <v>160560</v>
@@ -772,8 +775,8 @@
       <c r="B12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>11</v>
+      <c r="C12" s="1">
+        <v>175820</v>
       </c>
       <c r="D12">
         <v>175072</v>
@@ -802,10 +805,11 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>